<commit_message>
Working through the Lead Indicators report.
We need more data, and cleaner data too.
</commit_message>
<xml_diff>
--- a/ExcelDemoReports/2015 KPI Lead Indicators_July_original.xlsx
+++ b/ExcelDemoReports/2015 KPI Lead Indicators_July_original.xlsx
@@ -13394,9 +13394,9 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G8" sqref="G8"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>